<commit_message>
Update User Module - Add User and Assign Staff
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team12-TestData-LMS-UI-Hackathon-April2024.xlsx
+++ b/src/test/resources/TestData/Team12-TestData-LMS-UI-Hackathon-April2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amreennaziasyed/eclipse-workspace/DSALGO/Team12_XpathWarriors_LMS_UI_Apr2024/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CB68DE-4C9A-4949-A6EE-A86E356CAE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680CD73C-B6E9-494E-80A7-21C2E1ECFBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>First Name</t>
   </si>
@@ -133,7 +133,7 @@
     <t>xpathWarriors</t>
   </si>
   <si>
-    <t>xpathwarriors584@gmail.com</t>
+    <t>xpathwarriors588@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
         <v>36</v>
       </c>
       <c r="C2" s="1">
-        <v>7722334501</v>
+        <v>7722334502</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -606,6 +606,9 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O5" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="P5" s="1" t="s">
         <v>31</v>
       </c>
@@ -619,6 +622,9 @@
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="O6" s="2" t="s">
         <v>34</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>33</v>
@@ -633,6 +639,7 @@
     <hyperlink ref="J4" r:id="rId2" xr:uid="{0D3C8955-7B76-9A43-B5EE-5073F2B959F0}"/>
     <hyperlink ref="O6" r:id="rId3" xr:uid="{7C901519-D915-A948-A299-5A5B1DC454E3}"/>
     <hyperlink ref="J2" r:id="rId4" xr:uid="{0F40225D-D975-5645-BA5D-3CE8BDFB544E}"/>
+    <hyperlink ref="O5" r:id="rId5" xr:uid="{4AD94B83-DF25-1D45-AAFC-FD698BF5E3DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>